<commit_message>
add table loading anim + return-key-submit function
</commit_message>
<xml_diff>
--- a/Data/vocabulary.xlsx
+++ b/Data/vocabulary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitken/Documents/Personal/Chinese/Zhongwen/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D668CE-79B4-4044-BFFE-9DB09CA9114B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEA424D-7BD8-CF40-A640-A2F1723D9FA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{8B915728-1877-A945-B45F-7CFF5B7B066D}"/>
   </bookViews>
@@ -594,9 +594,6 @@
     <t>发</t>
   </si>
   <si>
-    <t>e-mail</t>
-  </si>
-  <si>
     <t>diànzǐ yóujiàn</t>
   </si>
   <si>
@@ -955,6 +952,9 @@
   </si>
   <si>
     <t>开水</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -1308,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B859B0ED-94BD-7D4F-8618-2055F3D8F45D}">
   <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1362,13 +1362,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C4" t="s">
         <v>249</v>
-      </c>
-      <c r="C4" t="s">
-        <v>250</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1913,13 +1913,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B44" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C44" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -1927,13 +1927,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>295</v>
+      </c>
+      <c r="B45" t="s">
         <v>296</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>297</v>
-      </c>
-      <c r="C45" t="s">
-        <v>298</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>189</v>
+      </c>
+      <c r="B69" t="s">
         <v>190</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>191</v>
-      </c>
-      <c r="C69" t="s">
-        <v>192</v>
       </c>
       <c r="D69">
         <v>2</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>192</v>
+      </c>
+      <c r="B70" t="s">
         <v>193</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>194</v>
-      </c>
-      <c r="C70" t="s">
-        <v>195</v>
       </c>
       <c r="D70">
         <v>2</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>307</v>
+      </c>
+      <c r="B71" t="s">
         <v>187</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>188</v>
-      </c>
-      <c r="C71" t="s">
-        <v>189</v>
       </c>
       <c r="D71">
         <v>2</v>
@@ -2302,7 +2302,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B72" t="s">
         <v>66</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>196</v>
+      </c>
+      <c r="B73" t="s">
         <v>197</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>198</v>
-      </c>
-      <c r="C73" t="s">
-        <v>199</v>
       </c>
       <c r="D73">
         <v>2</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>199</v>
+      </c>
+      <c r="B74" t="s">
         <v>200</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
         <v>201</v>
-      </c>
-      <c r="C74" t="s">
-        <v>202</v>
       </c>
       <c r="D74">
         <v>2</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>202</v>
+      </c>
+      <c r="B75" t="s">
         <v>203</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>204</v>
-      </c>
-      <c r="C75" t="s">
-        <v>205</v>
       </c>
       <c r="D75">
         <v>2</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>205</v>
+      </c>
+      <c r="B76" t="s">
         <v>206</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
         <v>207</v>
-      </c>
-      <c r="C76" t="s">
-        <v>208</v>
       </c>
       <c r="D76">
         <v>2</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>208</v>
+      </c>
+      <c r="B77" t="s">
         <v>209</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
         <v>210</v>
-      </c>
-      <c r="C77" t="s">
-        <v>211</v>
       </c>
       <c r="D77">
         <v>2</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>211</v>
+      </c>
+      <c r="B78" t="s">
         <v>212</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
         <v>213</v>
-      </c>
-      <c r="C78" t="s">
-        <v>214</v>
       </c>
       <c r="D78">
         <v>2</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>214</v>
+      </c>
+      <c r="B79" t="s">
         <v>215</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>216</v>
-      </c>
-      <c r="C79" t="s">
-        <v>217</v>
       </c>
       <c r="D79">
         <v>2</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>217</v>
+      </c>
+      <c r="B80" t="s">
         <v>218</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>219</v>
-      </c>
-      <c r="C80" t="s">
-        <v>220</v>
       </c>
       <c r="D80">
         <v>2</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B81" t="s">
+        <v>220</v>
+      </c>
+      <c r="C81" t="s">
         <v>221</v>
-      </c>
-      <c r="C81" t="s">
-        <v>222</v>
       </c>
       <c r="D81">
         <v>2</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B82" t="s">
+        <v>222</v>
+      </c>
+      <c r="C82" t="s">
         <v>223</v>
-      </c>
-      <c r="C82" t="s">
-        <v>224</v>
       </c>
       <c r="D82">
         <v>2</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>224</v>
+      </c>
+      <c r="B83" t="s">
         <v>225</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>226</v>
-      </c>
-      <c r="C83" t="s">
-        <v>227</v>
       </c>
       <c r="D83">
         <v>2</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B84" t="s">
+        <v>230</v>
+      </c>
+      <c r="C84" t="s">
         <v>231</v>
-      </c>
-      <c r="C84" t="s">
-        <v>232</v>
       </c>
       <c r="D84">
         <v>2</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>232</v>
+      </c>
+      <c r="B85" t="s">
         <v>233</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
         <v>234</v>
-      </c>
-      <c r="C85" t="s">
-        <v>235</v>
       </c>
       <c r="D85">
         <v>2</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>235</v>
+      </c>
+      <c r="B86" t="s">
         <v>236</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>237</v>
-      </c>
-      <c r="C86" t="s">
-        <v>238</v>
       </c>
       <c r="D86">
         <v>2</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>238</v>
+      </c>
+      <c r="B87" t="s">
         <v>239</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>240</v>
-      </c>
-      <c r="C87" t="s">
-        <v>241</v>
       </c>
       <c r="D87">
         <v>2</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>241</v>
+      </c>
+      <c r="B88" t="s">
         <v>242</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>243</v>
-      </c>
-      <c r="C88" t="s">
-        <v>244</v>
       </c>
       <c r="D88">
         <v>2</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>244</v>
+      </c>
+      <c r="B89" t="s">
         <v>245</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
         <v>246</v>
-      </c>
-      <c r="C89" t="s">
-        <v>247</v>
       </c>
       <c r="D89">
         <v>2</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B90" t="s">
+        <v>251</v>
+      </c>
+      <c r="C90" t="s">
         <v>252</v>
-      </c>
-      <c r="C90" t="s">
-        <v>253</v>
       </c>
       <c r="D90">
         <v>2</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>253</v>
+      </c>
+      <c r="B91" t="s">
         <v>254</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>255</v>
-      </c>
-      <c r="C91" t="s">
-        <v>256</v>
       </c>
       <c r="D91">
         <v>2</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>256</v>
+      </c>
+      <c r="B92" t="s">
         <v>257</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>258</v>
-      </c>
-      <c r="C92" t="s">
-        <v>259</v>
       </c>
       <c r="D92">
         <v>2</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>259</v>
+      </c>
+      <c r="B93" t="s">
+        <v>267</v>
+      </c>
+      <c r="C93" t="s">
         <v>260</v>
-      </c>
-      <c r="B93" t="s">
-        <v>268</v>
-      </c>
-      <c r="C93" t="s">
-        <v>261</v>
       </c>
       <c r="D93">
         <v>2</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>261</v>
+      </c>
+      <c r="B94" t="s">
         <v>262</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
         <v>263</v>
-      </c>
-      <c r="C94" t="s">
-        <v>264</v>
       </c>
       <c r="D94">
         <v>2</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>264</v>
+      </c>
+      <c r="B95" t="s">
         <v>265</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>266</v>
-      </c>
-      <c r="C95" t="s">
-        <v>267</v>
       </c>
       <c r="D95">
         <v>2</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>268</v>
+      </c>
+      <c r="B96" t="s">
         <v>269</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" t="s">
         <v>270</v>
-      </c>
-      <c r="C96" t="s">
-        <v>271</v>
       </c>
       <c r="D96">
         <v>2</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>271</v>
+      </c>
+      <c r="B97" t="s">
         <v>272</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
         <v>273</v>
-      </c>
-      <c r="C97" t="s">
-        <v>274</v>
       </c>
       <c r="D97">
         <v>2</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>274</v>
+      </c>
+      <c r="B98" t="s">
         <v>275</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
         <v>276</v>
-      </c>
-      <c r="C98" t="s">
-        <v>277</v>
       </c>
       <c r="D98">
         <v>2</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>277</v>
+      </c>
+      <c r="B99" t="s">
         <v>278</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
         <v>279</v>
-      </c>
-      <c r="C99" t="s">
-        <v>280</v>
       </c>
       <c r="D99">
         <v>2</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>280</v>
+      </c>
+      <c r="B100" t="s">
         <v>281</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>282</v>
-      </c>
-      <c r="C100" t="s">
-        <v>283</v>
       </c>
       <c r="D100">
         <v>2</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>283</v>
+      </c>
+      <c r="B101" t="s">
         <v>284</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
         <v>285</v>
-      </c>
-      <c r="C101" t="s">
-        <v>286</v>
       </c>
       <c r="D101">
         <v>2</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>286</v>
+      </c>
+      <c r="B102" t="s">
         <v>287</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
         <v>288</v>
-      </c>
-      <c r="C102" t="s">
-        <v>289</v>
       </c>
       <c r="D102">
         <v>2</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>289</v>
+      </c>
+      <c r="B103" t="s">
         <v>290</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
         <v>291</v>
-      </c>
-      <c r="C103" t="s">
-        <v>292</v>
       </c>
       <c r="D103">
         <v>2</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>292</v>
+      </c>
+      <c r="B104" t="s">
         <v>293</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
         <v>294</v>
-      </c>
-      <c r="C104" t="s">
-        <v>295</v>
       </c>
       <c r="D104">
         <v>2</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>301</v>
+      </c>
+      <c r="B105" t="s">
         <v>302</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>303</v>
-      </c>
-      <c r="C105" t="s">
-        <v>304</v>
       </c>
       <c r="D105">
         <v>2</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>304</v>
+      </c>
+      <c r="B106" t="s">
         <v>305</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
         <v>306</v>
-      </c>
-      <c r="C106" t="s">
-        <v>307</v>
       </c>
       <c r="D106">
         <v>2</v>

</xml_diff>

<commit_message>
add code to render cards containing key phrases
</commit_message>
<xml_diff>
--- a/Data/vocabulary.xlsx
+++ b/Data/vocabulary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitken/Documents/Personal/Chinese/Zhongwen/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEA424D-7BD8-CF40-A640-A2F1723D9FA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1369DCA4-70BE-FA46-AA69-B76FDDDB1CB5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{8B915728-1877-A945-B45F-7CFF5B7B066D}"/>
   </bookViews>
@@ -480,9 +480,6 @@
     <t>大学</t>
   </si>
   <si>
-    <t>department (of a university)</t>
-  </si>
-  <si>
     <t>xì</t>
   </si>
   <si>
@@ -955,6 +952,9 @@
   </si>
   <si>
     <t>email</t>
+  </si>
+  <si>
+    <t>department</t>
   </si>
 </sst>
 </file>
@@ -1308,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B859B0ED-94BD-7D4F-8618-2055F3D8F45D}">
   <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1362,13 +1362,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" t="s">
         <v>248</v>
-      </c>
-      <c r="C4" t="s">
-        <v>249</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1913,13 +1913,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B44" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C44" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -1927,13 +1927,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>294</v>
+      </c>
+      <c r="B45" t="s">
         <v>295</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>296</v>
-      </c>
-      <c r="C45" t="s">
-        <v>297</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -2081,13 +2081,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>307</v>
+      </c>
+      <c r="B56" t="s">
         <v>149</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>150</v>
-      </c>
-      <c r="C56" t="s">
-        <v>151</v>
       </c>
       <c r="D56">
         <v>2</v>
@@ -2095,13 +2095,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>151</v>
+      </c>
+      <c r="B57" t="s">
         <v>152</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>153</v>
-      </c>
-      <c r="C57" t="s">
-        <v>154</v>
       </c>
       <c r="D57">
         <v>2</v>
@@ -2109,13 +2109,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>154</v>
+      </c>
+      <c r="B58" t="s">
         <v>155</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>156</v>
-      </c>
-      <c r="C58" t="s">
-        <v>157</v>
       </c>
       <c r="D58">
         <v>2</v>
@@ -2123,13 +2123,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>157</v>
+      </c>
+      <c r="B59" t="s">
         <v>158</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>159</v>
-      </c>
-      <c r="C59" t="s">
-        <v>160</v>
       </c>
       <c r="D59">
         <v>2</v>
@@ -2137,13 +2137,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>163</v>
+      </c>
+      <c r="B60" t="s">
         <v>164</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>165</v>
-      </c>
-      <c r="C60" t="s">
-        <v>166</v>
       </c>
       <c r="D60">
         <v>2</v>
@@ -2151,13 +2151,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>160</v>
+      </c>
+      <c r="B61" t="s">
         <v>161</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>162</v>
-      </c>
-      <c r="C61" t="s">
-        <v>163</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -2165,13 +2165,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>166</v>
+      </c>
+      <c r="B62" t="s">
         <v>167</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>168</v>
-      </c>
-      <c r="C62" t="s">
-        <v>169</v>
       </c>
       <c r="D62">
         <v>2</v>
@@ -2179,10 +2179,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
+        <v>169</v>
+      </c>
+      <c r="C63" t="s">
         <v>170</v>
-      </c>
-      <c r="C63" t="s">
-        <v>171</v>
       </c>
       <c r="D63">
         <v>2</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>171</v>
+      </c>
+      <c r="B64" t="s">
         <v>172</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>173</v>
-      </c>
-      <c r="C64" t="s">
-        <v>174</v>
       </c>
       <c r="D64">
         <v>2</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>174</v>
+      </c>
+      <c r="B65" t="s">
         <v>175</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>176</v>
-      </c>
-      <c r="C65" t="s">
-        <v>177</v>
       </c>
       <c r="D65">
         <v>2</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>177</v>
+      </c>
+      <c r="B66" t="s">
         <v>178</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>179</v>
-      </c>
-      <c r="C66" t="s">
-        <v>180</v>
       </c>
       <c r="D66">
         <v>2</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>181</v>
+      </c>
+      <c r="B67" t="s">
+        <v>180</v>
+      </c>
+      <c r="C67" t="s">
         <v>182</v>
-      </c>
-      <c r="B67" t="s">
-        <v>181</v>
-      </c>
-      <c r="C67" t="s">
-        <v>183</v>
       </c>
       <c r="D67">
         <v>2</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>183</v>
+      </c>
+      <c r="B68" t="s">
         <v>184</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>185</v>
-      </c>
-      <c r="C68" t="s">
-        <v>186</v>
       </c>
       <c r="D68">
         <v>2</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>188</v>
+      </c>
+      <c r="B69" t="s">
         <v>189</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>190</v>
-      </c>
-      <c r="C69" t="s">
-        <v>191</v>
       </c>
       <c r="D69">
         <v>2</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>191</v>
+      </c>
+      <c r="B70" t="s">
         <v>192</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>193</v>
-      </c>
-      <c r="C70" t="s">
-        <v>194</v>
       </c>
       <c r="D70">
         <v>2</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B71" t="s">
+        <v>186</v>
+      </c>
+      <c r="C71" t="s">
         <v>187</v>
-      </c>
-      <c r="C71" t="s">
-        <v>188</v>
       </c>
       <c r="D71">
         <v>2</v>
@@ -2302,7 +2302,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B72" t="s">
         <v>66</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>195</v>
+      </c>
+      <c r="B73" t="s">
         <v>196</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>197</v>
-      </c>
-      <c r="C73" t="s">
-        <v>198</v>
       </c>
       <c r="D73">
         <v>2</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>198</v>
+      </c>
+      <c r="B74" t="s">
         <v>199</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
         <v>200</v>
-      </c>
-      <c r="C74" t="s">
-        <v>201</v>
       </c>
       <c r="D74">
         <v>2</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>201</v>
+      </c>
+      <c r="B75" t="s">
         <v>202</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>203</v>
-      </c>
-      <c r="C75" t="s">
-        <v>204</v>
       </c>
       <c r="D75">
         <v>2</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>204</v>
+      </c>
+      <c r="B76" t="s">
         <v>205</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
         <v>206</v>
-      </c>
-      <c r="C76" t="s">
-        <v>207</v>
       </c>
       <c r="D76">
         <v>2</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>207</v>
+      </c>
+      <c r="B77" t="s">
         <v>208</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
         <v>209</v>
-      </c>
-      <c r="C77" t="s">
-        <v>210</v>
       </c>
       <c r="D77">
         <v>2</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>210</v>
+      </c>
+      <c r="B78" t="s">
         <v>211</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
         <v>212</v>
-      </c>
-      <c r="C78" t="s">
-        <v>213</v>
       </c>
       <c r="D78">
         <v>2</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>213</v>
+      </c>
+      <c r="B79" t="s">
         <v>214</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>215</v>
-      </c>
-      <c r="C79" t="s">
-        <v>216</v>
       </c>
       <c r="D79">
         <v>2</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>216</v>
+      </c>
+      <c r="B80" t="s">
         <v>217</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>218</v>
-      </c>
-      <c r="C80" t="s">
-        <v>219</v>
       </c>
       <c r="D80">
         <v>2</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B81" t="s">
+        <v>219</v>
+      </c>
+      <c r="C81" t="s">
         <v>220</v>
-      </c>
-      <c r="C81" t="s">
-        <v>221</v>
       </c>
       <c r="D81">
         <v>2</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B82" t="s">
+        <v>221</v>
+      </c>
+      <c r="C82" t="s">
         <v>222</v>
-      </c>
-      <c r="C82" t="s">
-        <v>223</v>
       </c>
       <c r="D82">
         <v>2</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>223</v>
+      </c>
+      <c r="B83" t="s">
         <v>224</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>225</v>
-      </c>
-      <c r="C83" t="s">
-        <v>226</v>
       </c>
       <c r="D83">
         <v>2</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B84" t="s">
+        <v>229</v>
+      </c>
+      <c r="C84" t="s">
         <v>230</v>
-      </c>
-      <c r="C84" t="s">
-        <v>231</v>
       </c>
       <c r="D84">
         <v>2</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>231</v>
+      </c>
+      <c r="B85" t="s">
         <v>232</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
         <v>233</v>
-      </c>
-      <c r="C85" t="s">
-        <v>234</v>
       </c>
       <c r="D85">
         <v>2</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>234</v>
+      </c>
+      <c r="B86" t="s">
         <v>235</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>236</v>
-      </c>
-      <c r="C86" t="s">
-        <v>237</v>
       </c>
       <c r="D86">
         <v>2</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>237</v>
+      </c>
+      <c r="B87" t="s">
         <v>238</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>239</v>
-      </c>
-      <c r="C87" t="s">
-        <v>240</v>
       </c>
       <c r="D87">
         <v>2</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>240</v>
+      </c>
+      <c r="B88" t="s">
         <v>241</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>242</v>
-      </c>
-      <c r="C88" t="s">
-        <v>243</v>
       </c>
       <c r="D88">
         <v>2</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>243</v>
+      </c>
+      <c r="B89" t="s">
         <v>244</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
         <v>245</v>
-      </c>
-      <c r="C89" t="s">
-        <v>246</v>
       </c>
       <c r="D89">
         <v>2</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B90" t="s">
+        <v>250</v>
+      </c>
+      <c r="C90" t="s">
         <v>251</v>
-      </c>
-      <c r="C90" t="s">
-        <v>252</v>
       </c>
       <c r="D90">
         <v>2</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>252</v>
+      </c>
+      <c r="B91" t="s">
         <v>253</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>254</v>
-      </c>
-      <c r="C91" t="s">
-        <v>255</v>
       </c>
       <c r="D91">
         <v>2</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>255</v>
+      </c>
+      <c r="B92" t="s">
         <v>256</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>257</v>
-      </c>
-      <c r="C92" t="s">
-        <v>258</v>
       </c>
       <c r="D92">
         <v>2</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>258</v>
+      </c>
+      <c r="B93" t="s">
+        <v>266</v>
+      </c>
+      <c r="C93" t="s">
         <v>259</v>
-      </c>
-      <c r="B93" t="s">
-        <v>267</v>
-      </c>
-      <c r="C93" t="s">
-        <v>260</v>
       </c>
       <c r="D93">
         <v>2</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>260</v>
+      </c>
+      <c r="B94" t="s">
         <v>261</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
         <v>262</v>
-      </c>
-      <c r="C94" t="s">
-        <v>263</v>
       </c>
       <c r="D94">
         <v>2</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>263</v>
+      </c>
+      <c r="B95" t="s">
         <v>264</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>265</v>
-      </c>
-      <c r="C95" t="s">
-        <v>266</v>
       </c>
       <c r="D95">
         <v>2</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>267</v>
+      </c>
+      <c r="B96" t="s">
         <v>268</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" t="s">
         <v>269</v>
-      </c>
-      <c r="C96" t="s">
-        <v>270</v>
       </c>
       <c r="D96">
         <v>2</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>270</v>
+      </c>
+      <c r="B97" t="s">
         <v>271</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
         <v>272</v>
-      </c>
-      <c r="C97" t="s">
-        <v>273</v>
       </c>
       <c r="D97">
         <v>2</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>273</v>
+      </c>
+      <c r="B98" t="s">
         <v>274</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
         <v>275</v>
-      </c>
-      <c r="C98" t="s">
-        <v>276</v>
       </c>
       <c r="D98">
         <v>2</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>276</v>
+      </c>
+      <c r="B99" t="s">
         <v>277</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
         <v>278</v>
-      </c>
-      <c r="C99" t="s">
-        <v>279</v>
       </c>
       <c r="D99">
         <v>2</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>279</v>
+      </c>
+      <c r="B100" t="s">
         <v>280</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>281</v>
-      </c>
-      <c r="C100" t="s">
-        <v>282</v>
       </c>
       <c r="D100">
         <v>2</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>282</v>
+      </c>
+      <c r="B101" t="s">
         <v>283</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
         <v>284</v>
-      </c>
-      <c r="C101" t="s">
-        <v>285</v>
       </c>
       <c r="D101">
         <v>2</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>285</v>
+      </c>
+      <c r="B102" t="s">
         <v>286</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
         <v>287</v>
-      </c>
-      <c r="C102" t="s">
-        <v>288</v>
       </c>
       <c r="D102">
         <v>2</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>288</v>
+      </c>
+      <c r="B103" t="s">
         <v>289</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
         <v>290</v>
-      </c>
-      <c r="C103" t="s">
-        <v>291</v>
       </c>
       <c r="D103">
         <v>2</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>291</v>
+      </c>
+      <c r="B104" t="s">
         <v>292</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
         <v>293</v>
-      </c>
-      <c r="C104" t="s">
-        <v>294</v>
       </c>
       <c r="D104">
         <v>2</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>300</v>
+      </c>
+      <c r="B105" t="s">
         <v>301</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>302</v>
-      </c>
-      <c r="C105" t="s">
-        <v>303</v>
       </c>
       <c r="D105">
         <v>2</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>303</v>
+      </c>
+      <c r="B106" t="s">
         <v>304</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
         <v>305</v>
-      </c>
-      <c r="C106" t="s">
-        <v>306</v>
       </c>
       <c r="D106">
         <v>2</v>

</xml_diff>

<commit_message>
upload new vocabulary and hasten spinner fadeout
</commit_message>
<xml_diff>
--- a/Data/vocabulary.xlsx
+++ b/Data/vocabulary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitken/Documents/Personal/Chinese/Zhongwen/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1369DCA4-70BE-FA46-AA69-B76FDDDB1CB5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0586ACAD-1A7D-1F47-99AE-230BA26874DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{8B915728-1877-A945-B45F-7CFF5B7B066D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="593">
   <si>
     <t>you</t>
   </si>
@@ -114,9 +114,6 @@
     <t>们</t>
   </si>
   <si>
-    <t>teacher</t>
-  </si>
-  <si>
     <t>lǎoshī</t>
   </si>
   <si>
@@ -198,9 +195,6 @@
     <t>说</t>
   </si>
   <si>
-    <t>English (language)</t>
-  </si>
-  <si>
     <t>英语</t>
   </si>
   <si>
@@ -213,9 +207,6 @@
     <t>还是</t>
   </si>
   <si>
-    <t>French (language)</t>
-  </si>
-  <si>
     <t>法语</t>
   </si>
   <si>
@@ -252,9 +243,6 @@
     <t>he, him</t>
   </si>
   <si>
-    <t>tā</t>
-  </si>
-  <si>
     <t>他</t>
   </si>
   <si>
@@ -273,12 +261,6 @@
     <t>Australia</t>
   </si>
   <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
     <t>Russia</t>
   </si>
   <si>
@@ -300,9 +282,6 @@
     <t>中文</t>
   </si>
   <si>
-    <t>Chinese (language)</t>
-  </si>
-  <si>
     <t>Yīngwén</t>
   </si>
   <si>
@@ -955,6 +934,882 @@
   </si>
   <si>
     <t>department</t>
+  </si>
+  <si>
+    <t>English (yǔ - variant)</t>
+  </si>
+  <si>
+    <t>English (wén - variant)</t>
+  </si>
+  <si>
+    <t>French (yǔ - variant)</t>
+  </si>
+  <si>
+    <t>Chinese (yǔ - variant)</t>
+  </si>
+  <si>
+    <t>French (wén - variant)</t>
+  </si>
+  <si>
+    <t>Chinese (wén - variant)</t>
+  </si>
+  <si>
+    <t>tā (male)</t>
+  </si>
+  <si>
+    <t>tā (female)</t>
+  </si>
+  <si>
+    <t>United Kingdom, UK</t>
+  </si>
+  <si>
+    <t>United States, USA, US</t>
+  </si>
+  <si>
+    <t>这</t>
+  </si>
+  <si>
+    <t>zhè</t>
+  </si>
+  <si>
+    <t>place</t>
+  </si>
+  <si>
+    <t>dìfang</t>
+  </si>
+  <si>
+    <t>gè</t>
+  </si>
+  <si>
+    <t>zhèr</t>
+  </si>
+  <si>
+    <t>here (northern inflection)</t>
+  </si>
+  <si>
+    <t>here (southern inflection)</t>
+  </si>
+  <si>
+    <t>zhèli</t>
+  </si>
+  <si>
+    <t>family, home</t>
+  </si>
+  <si>
+    <t>jiā</t>
+  </si>
+  <si>
+    <t>have, there be</t>
+  </si>
+  <si>
+    <t>yǒu</t>
+  </si>
+  <si>
+    <t>how many</t>
+  </si>
+  <si>
+    <t>jǐ</t>
+  </si>
+  <si>
+    <t>kǒu</t>
+  </si>
+  <si>
+    <t>father</t>
+  </si>
+  <si>
+    <t>bàba</t>
+  </si>
+  <si>
+    <t>mother</t>
+  </si>
+  <si>
+    <t>māma</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>hé</t>
+  </si>
+  <si>
+    <t>wife</t>
+  </si>
+  <si>
+    <t>tàitai</t>
+  </si>
+  <si>
+    <t>child</t>
+  </si>
+  <si>
+    <t>háizi</t>
+  </si>
+  <si>
+    <t>boy</t>
+  </si>
+  <si>
+    <t>nánháir</t>
+  </si>
+  <si>
+    <t>girl</t>
+  </si>
+  <si>
+    <t>nǚháir</t>
+  </si>
+  <si>
+    <t>how old</t>
+  </si>
+  <si>
+    <t>duō dà</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>liǎng</t>
+  </si>
+  <si>
+    <t>two years old</t>
+  </si>
+  <si>
+    <t>liǎng suì</t>
+  </si>
+  <si>
+    <t>lovely, cute</t>
+  </si>
+  <si>
+    <t>kě'ài</t>
+  </si>
+  <si>
+    <t>ba</t>
+  </si>
+  <si>
+    <t>school</t>
+  </si>
+  <si>
+    <t>xuéxiào</t>
+  </si>
+  <si>
+    <t>how many, how much</t>
+  </si>
+  <si>
+    <t>duōshao</t>
+  </si>
+  <si>
+    <t>student</t>
+  </si>
+  <si>
+    <t>xuésheng</t>
+  </si>
+  <si>
+    <t>xiǎng</t>
+  </si>
+  <si>
+    <t>maybe, about</t>
+  </si>
+  <si>
+    <t>dàgài</t>
+  </si>
+  <si>
+    <t>ten thousand</t>
+  </si>
+  <si>
+    <t>wàn</t>
+  </si>
+  <si>
+    <t>not have</t>
+  </si>
+  <si>
+    <t>méiyǒu</t>
+  </si>
+  <si>
+    <t>many, much</t>
+  </si>
+  <si>
+    <t>duō</t>
+  </si>
+  <si>
+    <t>thousand</t>
+  </si>
+  <si>
+    <t>qiān</t>
+  </si>
+  <si>
+    <t>go</t>
+  </si>
+  <si>
+    <t>qù</t>
+  </si>
+  <si>
+    <t>why</t>
+  </si>
+  <si>
+    <t>wèi shénme</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t>wèi</t>
+  </si>
+  <si>
+    <t>branch of a company</t>
+  </si>
+  <si>
+    <t>fēngōngsī</t>
+  </si>
+  <si>
+    <t>boss</t>
+  </si>
+  <si>
+    <t>lǎobǎn</t>
+  </si>
+  <si>
+    <t>let</t>
+  </si>
+  <si>
+    <t>ràng</t>
+  </si>
+  <si>
+    <t>there (northern inflection)</t>
+  </si>
+  <si>
+    <t>nàr</t>
+  </si>
+  <si>
+    <t>there (southern inflection)</t>
+  </si>
+  <si>
+    <t>nàli</t>
+  </si>
+  <si>
+    <t>hundred</t>
+  </si>
+  <si>
+    <t>bǎi</t>
+  </si>
+  <si>
+    <t>few, little</t>
+  </si>
+  <si>
+    <t>shǎo</t>
+  </si>
+  <si>
+    <t>because</t>
+  </si>
+  <si>
+    <t>yīnwèi</t>
+  </si>
+  <si>
+    <t>地方</t>
+  </si>
+  <si>
+    <t>个</t>
+  </si>
+  <si>
+    <t>这儿</t>
+  </si>
+  <si>
+    <t>这里</t>
+  </si>
+  <si>
+    <t>家</t>
+  </si>
+  <si>
+    <t>有</t>
+  </si>
+  <si>
+    <t>几</t>
+  </si>
+  <si>
+    <t>口</t>
+  </si>
+  <si>
+    <t>爸爸</t>
+  </si>
+  <si>
+    <t>妈妈</t>
+  </si>
+  <si>
+    <t>和</t>
+  </si>
+  <si>
+    <t>太太</t>
+  </si>
+  <si>
+    <t>孩子</t>
+  </si>
+  <si>
+    <t>男孩儿</t>
+  </si>
+  <si>
+    <t>女孩儿</t>
+  </si>
+  <si>
+    <t>多大</t>
+  </si>
+  <si>
+    <t>两</t>
+  </si>
+  <si>
+    <t>两岁</t>
+  </si>
+  <si>
+    <t>可爱</t>
+  </si>
+  <si>
+    <t>吧</t>
+  </si>
+  <si>
+    <t>学校</t>
+  </si>
+  <si>
+    <t>多少</t>
+  </si>
+  <si>
+    <t>学生</t>
+  </si>
+  <si>
+    <t>想</t>
+  </si>
+  <si>
+    <t>大概</t>
+  </si>
+  <si>
+    <t>万</t>
+  </si>
+  <si>
+    <t>没有</t>
+  </si>
+  <si>
+    <t>多</t>
+  </si>
+  <si>
+    <t>千</t>
+  </si>
+  <si>
+    <t>去</t>
+  </si>
+  <si>
+    <t>为什么</t>
+  </si>
+  <si>
+    <t>分公司</t>
+  </si>
+  <si>
+    <t>为</t>
+  </si>
+  <si>
+    <t>老板</t>
+  </si>
+  <si>
+    <t>让</t>
+  </si>
+  <si>
+    <t>百</t>
+  </si>
+  <si>
+    <t>少</t>
+  </si>
+  <si>
+    <t>因为</t>
+  </si>
+  <si>
+    <t>husband</t>
+  </si>
+  <si>
+    <t>xiānsheng</t>
+  </si>
+  <si>
+    <t>gēge</t>
+  </si>
+  <si>
+    <t>elder brother</t>
+  </si>
+  <si>
+    <t>elder sister</t>
+  </si>
+  <si>
+    <t>jiějie</t>
+  </si>
+  <si>
+    <t>younger brother</t>
+  </si>
+  <si>
+    <t>dìdi</t>
+  </si>
+  <si>
+    <t>younger sister</t>
+  </si>
+  <si>
+    <t>mèimei</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>niánjì</t>
+  </si>
+  <si>
+    <t>(a) hundred million</t>
+  </si>
+  <si>
+    <t>yì</t>
+  </si>
+  <si>
+    <t>come</t>
+  </si>
+  <si>
+    <t>lái</t>
+  </si>
+  <si>
+    <t>employee</t>
+  </si>
+  <si>
+    <t>zhíyuán</t>
+  </si>
+  <si>
+    <t>先生</t>
+  </si>
+  <si>
+    <t>哥哥</t>
+  </si>
+  <si>
+    <t>姐姐</t>
+  </si>
+  <si>
+    <t>弟弟</t>
+  </si>
+  <si>
+    <t>妹妹</t>
+  </si>
+  <si>
+    <t>年纪</t>
+  </si>
+  <si>
+    <t>亿</t>
+  </si>
+  <si>
+    <t>来</t>
+  </si>
+  <si>
+    <t>职员</t>
+  </si>
+  <si>
+    <t>map</t>
+  </si>
+  <si>
+    <t>dìtú</t>
+  </si>
+  <si>
+    <t>zhāng</t>
+  </si>
+  <si>
+    <t>look</t>
+  </si>
+  <si>
+    <t>kàn</t>
+  </si>
+  <si>
+    <t>yíxià</t>
+  </si>
+  <si>
+    <t>xíng</t>
+  </si>
+  <si>
+    <t>ok, all right</t>
+  </si>
+  <si>
+    <t>think, want (to do something)</t>
+  </si>
+  <si>
+    <t>want (something/to do something)</t>
+  </si>
+  <si>
+    <t>yào</t>
+  </si>
+  <si>
+    <t>give</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>gàn</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>shìde</t>
+  </si>
+  <si>
+    <t>play, (do something) for pleasure</t>
+  </si>
+  <si>
+    <t>wánr</t>
+  </si>
+  <si>
+    <t>zhīdao</t>
+  </si>
+  <si>
+    <t>comparatively, relatively, fairly</t>
+  </si>
+  <si>
+    <t>bǐjiào</t>
+  </si>
+  <si>
+    <t>really</t>
+  </si>
+  <si>
+    <t>zhēn</t>
+  </si>
+  <si>
+    <t>interesting</t>
+  </si>
+  <si>
+    <t>yǒu yìsi</t>
+  </si>
+  <si>
+    <t>meaning</t>
+  </si>
+  <si>
+    <t>yìsi</t>
+  </si>
+  <si>
+    <t>dragon</t>
+  </si>
+  <si>
+    <t>lóng</t>
+  </si>
+  <si>
+    <t>mountain, hill</t>
+  </si>
+  <si>
+    <t>shān</t>
+  </si>
+  <si>
+    <t>dictionary</t>
+  </si>
+  <si>
+    <t>cídiǎn</t>
+  </si>
+  <si>
+    <t>Chinese-English dictionary</t>
+  </si>
+  <si>
+    <t>Hàn-Yīng cídiǎn</t>
+  </si>
+  <si>
+    <t>English-Chinese dictionary</t>
+  </si>
+  <si>
+    <t>Yīng-Hàn cídiǎn</t>
+  </si>
+  <si>
+    <t>běn</t>
+  </si>
+  <si>
+    <t>who</t>
+  </si>
+  <si>
+    <t>shuí</t>
+  </si>
+  <si>
+    <t>excuse me</t>
+  </si>
+  <si>
+    <t>qǐng wèn</t>
+  </si>
+  <si>
+    <t>ask</t>
+  </si>
+  <si>
+    <t>wèn</t>
+  </si>
+  <si>
+    <t>correct, yes</t>
+  </si>
+  <si>
+    <t>duì</t>
+  </si>
+  <si>
+    <t>very, very much</t>
+  </si>
+  <si>
+    <t>fēicháng</t>
+  </si>
+  <si>
+    <t>useful</t>
+  </si>
+  <si>
+    <t>yǒuyòng</t>
+  </si>
+  <si>
+    <t>can</t>
+  </si>
+  <si>
+    <t>néng</t>
+  </si>
+  <si>
+    <t>use</t>
+  </si>
+  <si>
+    <t>yòng</t>
+  </si>
+  <si>
+    <t>of course</t>
+  </si>
+  <si>
+    <t>dāngrán</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>shū</t>
+  </si>
+  <si>
+    <t>notebook</t>
+  </si>
+  <si>
+    <t>běnzi</t>
+  </si>
+  <si>
+    <t>pen</t>
+  </si>
+  <si>
+    <t>bǐ</t>
+  </si>
+  <si>
+    <t>zhī</t>
+  </si>
+  <si>
+    <t>classroom</t>
+  </si>
+  <si>
+    <t>jiàoshì</t>
+  </si>
+  <si>
+    <t>attend class</t>
+  </si>
+  <si>
+    <t>shàng kè</t>
+  </si>
+  <si>
+    <t>Beijing</t>
+  </si>
+  <si>
+    <t>Shanghai</t>
+  </si>
+  <si>
+    <t>Shànghǎi</t>
+  </si>
+  <si>
+    <t>Běijīng</t>
+  </si>
+  <si>
+    <t>Longshan</t>
+  </si>
+  <si>
+    <t>Lóngshān</t>
+  </si>
+  <si>
+    <t>textbook</t>
+  </si>
+  <si>
+    <t>kèběn</t>
+  </si>
+  <si>
+    <t>recorder</t>
+  </si>
+  <si>
+    <t>lùxiàngjī</t>
+  </si>
+  <si>
+    <t>lùyīnjī</t>
+  </si>
+  <si>
+    <t>VCR</t>
+  </si>
+  <si>
+    <t>tái</t>
+  </si>
+  <si>
+    <t>tape</t>
+  </si>
+  <si>
+    <t>cídài</t>
+  </si>
+  <si>
+    <t>video tape</t>
+  </si>
+  <si>
+    <t>lùxiàngdài</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>guāngpán</t>
+  </si>
+  <si>
+    <t>teacher (formal)</t>
+  </si>
+  <si>
+    <t>teacher (informal)</t>
+  </si>
+  <si>
+    <t>jiàoshī</t>
+  </si>
+  <si>
+    <t>blackboard</t>
+  </si>
+  <si>
+    <t>hēibǎn</t>
+  </si>
+  <si>
+    <t>地图</t>
+  </si>
+  <si>
+    <t>张</t>
+  </si>
+  <si>
+    <t>看</t>
+  </si>
+  <si>
+    <t>一下</t>
+  </si>
+  <si>
+    <t>行</t>
+  </si>
+  <si>
+    <t>要</t>
+  </si>
+  <si>
+    <t>gěi (verb)</t>
+  </si>
+  <si>
+    <t>给 (verb)</t>
+  </si>
+  <si>
+    <t>干</t>
+  </si>
+  <si>
+    <t>是的</t>
+  </si>
+  <si>
+    <t>玩儿</t>
+  </si>
+  <si>
+    <t>知道</t>
+  </si>
+  <si>
+    <t>比较</t>
+  </si>
+  <si>
+    <t>真</t>
+  </si>
+  <si>
+    <t>有意思</t>
+  </si>
+  <si>
+    <t>意思</t>
+  </si>
+  <si>
+    <t>龙</t>
+  </si>
+  <si>
+    <t>山</t>
+  </si>
+  <si>
+    <t>词典</t>
+  </si>
+  <si>
+    <t>汉英词典</t>
+  </si>
+  <si>
+    <t>英汉词典</t>
+  </si>
+  <si>
+    <t>本</t>
+  </si>
+  <si>
+    <t>谁</t>
+  </si>
+  <si>
+    <t>请问</t>
+  </si>
+  <si>
+    <t>问</t>
+  </si>
+  <si>
+    <t>对</t>
+  </si>
+  <si>
+    <t>非常</t>
+  </si>
+  <si>
+    <t>有用</t>
+  </si>
+  <si>
+    <t>能</t>
+  </si>
+  <si>
+    <t>用</t>
+  </si>
+  <si>
+    <t>当然</t>
+  </si>
+  <si>
+    <t>书</t>
+  </si>
+  <si>
+    <t>本子</t>
+  </si>
+  <si>
+    <t>笔</t>
+  </si>
+  <si>
+    <t>支</t>
+  </si>
+  <si>
+    <t>教师</t>
+  </si>
+  <si>
+    <t>上课</t>
+  </si>
+  <si>
+    <t>北京</t>
+  </si>
+  <si>
+    <t>上海</t>
+  </si>
+  <si>
+    <t>龙山</t>
+  </si>
+  <si>
+    <t>课本</t>
+  </si>
+  <si>
+    <t>录音机</t>
+  </si>
+  <si>
+    <t>拉相机</t>
+  </si>
+  <si>
+    <t>台</t>
+  </si>
+  <si>
+    <t>磁带</t>
+  </si>
+  <si>
+    <t>拉相待</t>
+  </si>
+  <si>
+    <t>光盘</t>
+  </si>
+  <si>
+    <t>黑板</t>
   </si>
 </sst>
 </file>
@@ -1306,30 +2161,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B859B0ED-94BD-7D4F-8618-2055F3D8F45D}">
-  <dimension ref="A1:D106"/>
+  <dimension ref="A1:D203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="185" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E200" sqref="E200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1362,13 +2217,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B4" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="C4" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1479,13 +2334,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>541</v>
+      </c>
+      <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1493,13 +2348,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1510,10 +2365,10 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
         <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1521,13 +2376,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
         <v>35</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>36</v>
-      </c>
-      <c r="C16" t="s">
-        <v>37</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1535,13 +2390,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>39</v>
-      </c>
-      <c r="C17" t="s">
-        <v>40</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1549,13 +2404,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>42</v>
-      </c>
-      <c r="C18" t="s">
-        <v>43</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1563,13 +2418,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
         <v>44</v>
       </c>
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
       <c r="C19" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1577,13 +2432,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
         <v>46</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>47</v>
-      </c>
-      <c r="C20" t="s">
-        <v>48</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1591,13 +2446,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
         <v>49</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>50</v>
-      </c>
-      <c r="C21" t="s">
-        <v>51</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1605,13 +2460,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
         <v>52</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>53</v>
-      </c>
-      <c r="C22" t="s">
-        <v>54</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1619,13 +2474,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>301</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1633,13 +2488,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>302</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1647,13 +2502,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
         <v>57</v>
-      </c>
-      <c r="B25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" t="s">
-        <v>59</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1661,13 +2516,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>303</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1675,13 +2530,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>305</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1689,13 +2544,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1703,13 +2558,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1717,13 +2572,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>304</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1731,13 +2586,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>306</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1745,13 +2600,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>307</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1759,13 +2614,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>308</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1773,13 +2628,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C34" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1787,13 +2642,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C35" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1801,13 +2656,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B36" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C36" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1815,13 +2670,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>310</v>
       </c>
       <c r="B37" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C37" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1829,13 +2684,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>309</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C38" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1843,13 +2698,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C39" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -1857,13 +2712,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C40" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1871,13 +2726,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -1885,13 +2740,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B42" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1899,13 +2754,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C43" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1913,13 +2768,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B44" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="C44" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -1927,13 +2782,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B45" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="C45" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1941,13 +2796,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C46" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D46">
         <v>2</v>
@@ -1955,13 +2810,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B47" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C47" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -1969,13 +2824,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B48" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C48" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D48">
         <v>2</v>
@@ -1983,13 +2838,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B49" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C49" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D49">
         <v>2</v>
@@ -1997,13 +2852,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B50" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C50" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D50">
         <v>2</v>
@@ -2011,13 +2866,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B51" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C51" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D51">
         <v>2</v>
@@ -2025,13 +2880,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B52" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C52" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D52">
         <v>2</v>
@@ -2039,13 +2894,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B53" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C53" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D53">
         <v>2</v>
@@ -2053,13 +2908,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B54" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C54" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D54">
         <v>2</v>
@@ -2067,13 +2922,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B55" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C55" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D55">
         <v>2</v>
@@ -2081,13 +2936,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="B56" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C56" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D56">
         <v>2</v>
@@ -2095,13 +2950,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B57" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C57" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D57">
         <v>2</v>
@@ -2109,13 +2964,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B58" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C58" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="D58">
         <v>2</v>
@@ -2123,13 +2978,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C59" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D59">
         <v>2</v>
@@ -2137,13 +2992,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B60" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C60" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D60">
         <v>2</v>
@@ -2151,13 +3006,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B61" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C61" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -2165,13 +3020,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B62" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C62" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D62">
         <v>2</v>
@@ -2179,10 +3034,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C63" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D63">
         <v>2</v>
@@ -2190,13 +3045,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B64" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C64" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D64">
         <v>2</v>
@@ -2204,13 +3059,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B65" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C65" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D65">
         <v>2</v>
@@ -2218,13 +3073,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B66" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C66" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D66">
         <v>2</v>
@@ -2232,13 +3087,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B67" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C67" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D67">
         <v>2</v>
@@ -2246,13 +3101,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B68" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C68" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D68">
         <v>2</v>
@@ -2260,13 +3115,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B69" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C69" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D69">
         <v>2</v>
@@ -2274,13 +3129,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B70" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C70" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D70">
         <v>2</v>
@@ -2288,13 +3143,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="B71" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C71" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D71">
         <v>2</v>
@@ -2302,13 +3157,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B72" t="s">
-        <v>66</v>
+        <v>312</v>
       </c>
       <c r="C72" t="s">
-        <v>67</v>
+        <v>311</v>
       </c>
       <c r="D72">
         <v>2</v>
@@ -2316,13 +3171,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B73" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C73" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D73">
         <v>2</v>
@@ -2330,13 +3185,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B74" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C74" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D74">
         <v>2</v>
@@ -2344,13 +3199,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B75" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C75" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D75">
         <v>2</v>
@@ -2358,13 +3213,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B76" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C76" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D76">
         <v>2</v>
@@ -2372,13 +3227,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B77" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C77" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D77">
         <v>2</v>
@@ -2386,13 +3241,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B78" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C78" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="D78">
         <v>2</v>
@@ -2400,13 +3255,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B79" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C79" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="D79">
         <v>2</v>
@@ -2414,13 +3269,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B80" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C80" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D80">
         <v>2</v>
@@ -2428,13 +3283,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B81" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C81" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D81">
         <v>2</v>
@@ -2442,13 +3297,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B82" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C82" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D82">
         <v>2</v>
@@ -2456,13 +3311,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B83" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C83" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D83">
         <v>2</v>
@@ -2470,13 +3325,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="B84" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C84" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D84">
         <v>2</v>
@@ -2484,13 +3339,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B85" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="C85" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="D85">
         <v>2</v>
@@ -2498,13 +3353,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B86" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C86" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D86">
         <v>2</v>
@@ -2512,13 +3367,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B87" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C87" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="D87">
         <v>2</v>
@@ -2526,13 +3381,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="B88" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="C88" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D88">
         <v>2</v>
@@ -2540,13 +3395,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B89" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="C89" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="D89">
         <v>2</v>
@@ -2554,13 +3409,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="B90" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C90" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D90">
         <v>2</v>
@@ -2568,13 +3423,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="B91" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C91" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="D91">
         <v>2</v>
@@ -2582,13 +3437,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B92" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C92" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D92">
         <v>2</v>
@@ -2596,13 +3451,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B93" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C93" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D93">
         <v>2</v>
@@ -2610,13 +3465,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="B94" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C94" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="D94">
         <v>2</v>
@@ -2624,13 +3479,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B95" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="C95" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="D95">
         <v>2</v>
@@ -2638,13 +3493,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="B96" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C96" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D96">
         <v>2</v>
@@ -2652,13 +3507,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="B97" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C97" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="D97">
         <v>2</v>
@@ -2666,13 +3521,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B98" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C98" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D98">
         <v>2</v>
@@ -2680,13 +3535,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="B99" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C99" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D99">
         <v>2</v>
@@ -2694,13 +3549,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="B100" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="C100" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="D100">
         <v>2</v>
@@ -2708,13 +3563,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B101" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="C101" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D101">
         <v>2</v>
@@ -2722,13 +3577,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="B102" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C102" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="D102">
         <v>2</v>
@@ -2736,13 +3591,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="B103" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C103" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D103">
         <v>2</v>
@@ -2750,13 +3605,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="B104" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="C104" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="D104">
         <v>2</v>
@@ -2764,13 +3619,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="B105" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="C105" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="D105">
         <v>2</v>
@@ -2778,16 +3633,1350 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="B106" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="C106" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D106">
         <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>313</v>
+      </c>
+      <c r="B107" t="s">
+        <v>314</v>
+      </c>
+      <c r="C107" t="s">
+        <v>389</v>
+      </c>
+      <c r="D107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B108" t="s">
+        <v>315</v>
+      </c>
+      <c r="C108" t="s">
+        <v>390</v>
+      </c>
+      <c r="D108">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>317</v>
+      </c>
+      <c r="B109" t="s">
+        <v>316</v>
+      </c>
+      <c r="C109" t="s">
+        <v>391</v>
+      </c>
+      <c r="D109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>318</v>
+      </c>
+      <c r="B110" t="s">
+        <v>319</v>
+      </c>
+      <c r="C110" t="s">
+        <v>392</v>
+      </c>
+      <c r="D110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>320</v>
+      </c>
+      <c r="B111" t="s">
+        <v>321</v>
+      </c>
+      <c r="C111" t="s">
+        <v>393</v>
+      </c>
+      <c r="D111">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>322</v>
+      </c>
+      <c r="B112" t="s">
+        <v>323</v>
+      </c>
+      <c r="C112" t="s">
+        <v>394</v>
+      </c>
+      <c r="D112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>324</v>
+      </c>
+      <c r="B113" t="s">
+        <v>325</v>
+      </c>
+      <c r="C113" t="s">
+        <v>395</v>
+      </c>
+      <c r="D113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
+        <v>326</v>
+      </c>
+      <c r="C114" t="s">
+        <v>396</v>
+      </c>
+      <c r="D114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>327</v>
+      </c>
+      <c r="B115" t="s">
+        <v>328</v>
+      </c>
+      <c r="C115" t="s">
+        <v>397</v>
+      </c>
+      <c r="D115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>329</v>
+      </c>
+      <c r="B116" t="s">
+        <v>330</v>
+      </c>
+      <c r="C116" t="s">
+        <v>398</v>
+      </c>
+      <c r="D116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>331</v>
+      </c>
+      <c r="B117" t="s">
+        <v>332</v>
+      </c>
+      <c r="C117" t="s">
+        <v>399</v>
+      </c>
+      <c r="D117">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>333</v>
+      </c>
+      <c r="B118" t="s">
+        <v>334</v>
+      </c>
+      <c r="C118" t="s">
+        <v>400</v>
+      </c>
+      <c r="D118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>335</v>
+      </c>
+      <c r="B119" t="s">
+        <v>336</v>
+      </c>
+      <c r="C119" t="s">
+        <v>401</v>
+      </c>
+      <c r="D119">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>337</v>
+      </c>
+      <c r="B120" t="s">
+        <v>338</v>
+      </c>
+      <c r="C120" t="s">
+        <v>402</v>
+      </c>
+      <c r="D120">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>339</v>
+      </c>
+      <c r="B121" t="s">
+        <v>340</v>
+      </c>
+      <c r="C121" t="s">
+        <v>403</v>
+      </c>
+      <c r="D121">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>341</v>
+      </c>
+      <c r="B122" t="s">
+        <v>342</v>
+      </c>
+      <c r="C122" t="s">
+        <v>404</v>
+      </c>
+      <c r="D122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>343</v>
+      </c>
+      <c r="B123" t="s">
+        <v>344</v>
+      </c>
+      <c r="C123" t="s">
+        <v>405</v>
+      </c>
+      <c r="D123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>345</v>
+      </c>
+      <c r="B124" t="s">
+        <v>346</v>
+      </c>
+      <c r="C124" t="s">
+        <v>406</v>
+      </c>
+      <c r="D124">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>347</v>
+      </c>
+      <c r="B125" t="s">
+        <v>348</v>
+      </c>
+      <c r="C125" t="s">
+        <v>407</v>
+      </c>
+      <c r="D125">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B126" t="s">
+        <v>349</v>
+      </c>
+      <c r="C126" t="s">
+        <v>408</v>
+      </c>
+      <c r="D126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>350</v>
+      </c>
+      <c r="B127" t="s">
+        <v>351</v>
+      </c>
+      <c r="C127" t="s">
+        <v>409</v>
+      </c>
+      <c r="D127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>352</v>
+      </c>
+      <c r="B128" t="s">
+        <v>353</v>
+      </c>
+      <c r="C128" t="s">
+        <v>410</v>
+      </c>
+      <c r="D128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>354</v>
+      </c>
+      <c r="B129" t="s">
+        <v>355</v>
+      </c>
+      <c r="C129" t="s">
+        <v>411</v>
+      </c>
+      <c r="D129">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>462</v>
+      </c>
+      <c r="B130" t="s">
+        <v>356</v>
+      </c>
+      <c r="C130" t="s">
+        <v>412</v>
+      </c>
+      <c r="D130">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>357</v>
+      </c>
+      <c r="B131" t="s">
+        <v>358</v>
+      </c>
+      <c r="C131" t="s">
+        <v>413</v>
+      </c>
+      <c r="D131">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>359</v>
+      </c>
+      <c r="B132" t="s">
+        <v>360</v>
+      </c>
+      <c r="C132" t="s">
+        <v>414</v>
+      </c>
+      <c r="D132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>361</v>
+      </c>
+      <c r="B133" t="s">
+        <v>362</v>
+      </c>
+      <c r="C133" t="s">
+        <v>415</v>
+      </c>
+      <c r="D133">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>363</v>
+      </c>
+      <c r="B134" t="s">
+        <v>364</v>
+      </c>
+      <c r="C134" t="s">
+        <v>416</v>
+      </c>
+      <c r="D134">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>365</v>
+      </c>
+      <c r="B135" t="s">
+        <v>366</v>
+      </c>
+      <c r="C135" t="s">
+        <v>417</v>
+      </c>
+      <c r="D135">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>367</v>
+      </c>
+      <c r="B136" t="s">
+        <v>368</v>
+      </c>
+      <c r="C136" t="s">
+        <v>418</v>
+      </c>
+      <c r="D136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>369</v>
+      </c>
+      <c r="B137" t="s">
+        <v>370</v>
+      </c>
+      <c r="C137" t="s">
+        <v>419</v>
+      </c>
+      <c r="D137">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>371</v>
+      </c>
+      <c r="B138" t="s">
+        <v>372</v>
+      </c>
+      <c r="C138" t="s">
+        <v>421</v>
+      </c>
+      <c r="D138">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>373</v>
+      </c>
+      <c r="B139" t="s">
+        <v>374</v>
+      </c>
+      <c r="C139" t="s">
+        <v>420</v>
+      </c>
+      <c r="D139">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>375</v>
+      </c>
+      <c r="B140" t="s">
+        <v>376</v>
+      </c>
+      <c r="C140" t="s">
+        <v>422</v>
+      </c>
+      <c r="D140">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>377</v>
+      </c>
+      <c r="B141" t="s">
+        <v>378</v>
+      </c>
+      <c r="C141" t="s">
+        <v>423</v>
+      </c>
+      <c r="D141">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>379</v>
+      </c>
+      <c r="B142" t="s">
+        <v>380</v>
+      </c>
+      <c r="C142" t="s">
+        <v>213</v>
+      </c>
+      <c r="D142">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>381</v>
+      </c>
+      <c r="B143" t="s">
+        <v>382</v>
+      </c>
+      <c r="C143" t="s">
+        <v>215</v>
+      </c>
+      <c r="D143">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>383</v>
+      </c>
+      <c r="B144" t="s">
+        <v>384</v>
+      </c>
+      <c r="C144" t="s">
+        <v>424</v>
+      </c>
+      <c r="D144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>385</v>
+      </c>
+      <c r="B145" t="s">
+        <v>386</v>
+      </c>
+      <c r="C145" t="s">
+        <v>425</v>
+      </c>
+      <c r="D145">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>387</v>
+      </c>
+      <c r="B146" t="s">
+        <v>388</v>
+      </c>
+      <c r="C146" t="s">
+        <v>426</v>
+      </c>
+      <c r="D146">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>427</v>
+      </c>
+      <c r="B147" t="s">
+        <v>428</v>
+      </c>
+      <c r="C147" t="s">
+        <v>445</v>
+      </c>
+      <c r="D147">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>430</v>
+      </c>
+      <c r="B148" t="s">
+        <v>429</v>
+      </c>
+      <c r="C148" t="s">
+        <v>446</v>
+      </c>
+      <c r="D148">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>431</v>
+      </c>
+      <c r="B149" t="s">
+        <v>432</v>
+      </c>
+      <c r="C149" t="s">
+        <v>447</v>
+      </c>
+      <c r="D149">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>433</v>
+      </c>
+      <c r="B150" t="s">
+        <v>434</v>
+      </c>
+      <c r="C150" t="s">
+        <v>448</v>
+      </c>
+      <c r="D150">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>435</v>
+      </c>
+      <c r="B151" t="s">
+        <v>436</v>
+      </c>
+      <c r="C151" t="s">
+        <v>449</v>
+      </c>
+      <c r="D151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>437</v>
+      </c>
+      <c r="B152" t="s">
+        <v>438</v>
+      </c>
+      <c r="C152" t="s">
+        <v>450</v>
+      </c>
+      <c r="D152">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>439</v>
+      </c>
+      <c r="B153" t="s">
+        <v>440</v>
+      </c>
+      <c r="C153" t="s">
+        <v>451</v>
+      </c>
+      <c r="D153">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>441</v>
+      </c>
+      <c r="B154" t="s">
+        <v>442</v>
+      </c>
+      <c r="C154" t="s">
+        <v>452</v>
+      </c>
+      <c r="D154">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>443</v>
+      </c>
+      <c r="B155" t="s">
+        <v>444</v>
+      </c>
+      <c r="C155" t="s">
+        <v>453</v>
+      </c>
+      <c r="D155">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>454</v>
+      </c>
+      <c r="B156" t="s">
+        <v>455</v>
+      </c>
+      <c r="C156" t="s">
+        <v>545</v>
+      </c>
+      <c r="D156">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B157" t="s">
+        <v>456</v>
+      </c>
+      <c r="C157" t="s">
+        <v>546</v>
+      </c>
+      <c r="D157">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>457</v>
+      </c>
+      <c r="B158" t="s">
+        <v>458</v>
+      </c>
+      <c r="C158" t="s">
+        <v>547</v>
+      </c>
+      <c r="D158">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B159" t="s">
+        <v>459</v>
+      </c>
+      <c r="C159" t="s">
+        <v>548</v>
+      </c>
+      <c r="D159">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>461</v>
+      </c>
+      <c r="B160" t="s">
+        <v>460</v>
+      </c>
+      <c r="C160" t="s">
+        <v>549</v>
+      </c>
+      <c r="D160">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>463</v>
+      </c>
+      <c r="B161" t="s">
+        <v>464</v>
+      </c>
+      <c r="C161" t="s">
+        <v>550</v>
+      </c>
+      <c r="D161">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>465</v>
+      </c>
+      <c r="B162" t="s">
+        <v>551</v>
+      </c>
+      <c r="C162" t="s">
+        <v>552</v>
+      </c>
+      <c r="D162">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>466</v>
+      </c>
+      <c r="B163" t="s">
+        <v>467</v>
+      </c>
+      <c r="C163" t="s">
+        <v>553</v>
+      </c>
+      <c r="D163">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>468</v>
+      </c>
+      <c r="B164" t="s">
+        <v>469</v>
+      </c>
+      <c r="C164" t="s">
+        <v>554</v>
+      </c>
+      <c r="D164">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>470</v>
+      </c>
+      <c r="B165" t="s">
+        <v>471</v>
+      </c>
+      <c r="C165" t="s">
+        <v>555</v>
+      </c>
+      <c r="D165">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>112</v>
+      </c>
+      <c r="B166" t="s">
+        <v>472</v>
+      </c>
+      <c r="C166" t="s">
+        <v>556</v>
+      </c>
+      <c r="D166">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>473</v>
+      </c>
+      <c r="B167" t="s">
+        <v>474</v>
+      </c>
+      <c r="C167" t="s">
+        <v>557</v>
+      </c>
+      <c r="D167">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>475</v>
+      </c>
+      <c r="B168" t="s">
+        <v>476</v>
+      </c>
+      <c r="C168" t="s">
+        <v>558</v>
+      </c>
+      <c r="D168">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>477</v>
+      </c>
+      <c r="B169" t="s">
+        <v>478</v>
+      </c>
+      <c r="C169" t="s">
+        <v>559</v>
+      </c>
+      <c r="D169">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>479</v>
+      </c>
+      <c r="B170" t="s">
+        <v>480</v>
+      </c>
+      <c r="C170" t="s">
+        <v>560</v>
+      </c>
+      <c r="D170">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>481</v>
+      </c>
+      <c r="B171" t="s">
+        <v>482</v>
+      </c>
+      <c r="C171" t="s">
+        <v>561</v>
+      </c>
+      <c r="D171">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>483</v>
+      </c>
+      <c r="B172" t="s">
+        <v>484</v>
+      </c>
+      <c r="C172" t="s">
+        <v>562</v>
+      </c>
+      <c r="D172">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>485</v>
+      </c>
+      <c r="B173" t="s">
+        <v>486</v>
+      </c>
+      <c r="C173" t="s">
+        <v>563</v>
+      </c>
+      <c r="D173">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>487</v>
+      </c>
+      <c r="B174" t="s">
+        <v>488</v>
+      </c>
+      <c r="C174" t="s">
+        <v>564</v>
+      </c>
+      <c r="D174">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>489</v>
+      </c>
+      <c r="B175" t="s">
+        <v>490</v>
+      </c>
+      <c r="C175" t="s">
+        <v>565</v>
+      </c>
+      <c r="D175">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B176" t="s">
+        <v>491</v>
+      </c>
+      <c r="C176" t="s">
+        <v>566</v>
+      </c>
+      <c r="D176">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>492</v>
+      </c>
+      <c r="B177" t="s">
+        <v>493</v>
+      </c>
+      <c r="C177" t="s">
+        <v>567</v>
+      </c>
+      <c r="D177">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>494</v>
+      </c>
+      <c r="B178" t="s">
+        <v>495</v>
+      </c>
+      <c r="C178" t="s">
+        <v>568</v>
+      </c>
+      <c r="D178">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>496</v>
+      </c>
+      <c r="B179" t="s">
+        <v>497</v>
+      </c>
+      <c r="C179" t="s">
+        <v>569</v>
+      </c>
+      <c r="D179">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>498</v>
+      </c>
+      <c r="B180" t="s">
+        <v>499</v>
+      </c>
+      <c r="C180" t="s">
+        <v>570</v>
+      </c>
+      <c r="D180">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>500</v>
+      </c>
+      <c r="B181" t="s">
+        <v>501</v>
+      </c>
+      <c r="C181" t="s">
+        <v>571</v>
+      </c>
+      <c r="D181">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>502</v>
+      </c>
+      <c r="B182" t="s">
+        <v>503</v>
+      </c>
+      <c r="C182" t="s">
+        <v>572</v>
+      </c>
+      <c r="D182">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>504</v>
+      </c>
+      <c r="B183" t="s">
+        <v>505</v>
+      </c>
+      <c r="C183" t="s">
+        <v>573</v>
+      </c>
+      <c r="D183">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>506</v>
+      </c>
+      <c r="B184" t="s">
+        <v>507</v>
+      </c>
+      <c r="C184" t="s">
+        <v>574</v>
+      </c>
+      <c r="D184">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>508</v>
+      </c>
+      <c r="B185" t="s">
+        <v>509</v>
+      </c>
+      <c r="C185" t="s">
+        <v>575</v>
+      </c>
+      <c r="D185">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>510</v>
+      </c>
+      <c r="B186" t="s">
+        <v>511</v>
+      </c>
+      <c r="C186" t="s">
+        <v>576</v>
+      </c>
+      <c r="D186">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>512</v>
+      </c>
+      <c r="B187" t="s">
+        <v>513</v>
+      </c>
+      <c r="C187" t="s">
+        <v>577</v>
+      </c>
+      <c r="D187">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>514</v>
+      </c>
+      <c r="B188" t="s">
+        <v>515</v>
+      </c>
+      <c r="C188" t="s">
+        <v>578</v>
+      </c>
+      <c r="D188">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B189" t="s">
+        <v>516</v>
+      </c>
+      <c r="C189" t="s">
+        <v>579</v>
+      </c>
+      <c r="D189">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>517</v>
+      </c>
+      <c r="B190" t="s">
+        <v>518</v>
+      </c>
+      <c r="C190" t="s">
+        <v>580</v>
+      </c>
+      <c r="D190">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>519</v>
+      </c>
+      <c r="B191" t="s">
+        <v>520</v>
+      </c>
+      <c r="C191" t="s">
+        <v>581</v>
+      </c>
+      <c r="D191">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>521</v>
+      </c>
+      <c r="B192" t="s">
+        <v>524</v>
+      </c>
+      <c r="C192" t="s">
+        <v>582</v>
+      </c>
+      <c r="D192">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>522</v>
+      </c>
+      <c r="B193" t="s">
+        <v>523</v>
+      </c>
+      <c r="C193" t="s">
+        <v>583</v>
+      </c>
+      <c r="D193">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>525</v>
+      </c>
+      <c r="B194" t="s">
+        <v>526</v>
+      </c>
+      <c r="C194" t="s">
+        <v>584</v>
+      </c>
+      <c r="D194">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>527</v>
+      </c>
+      <c r="B195" t="s">
+        <v>528</v>
+      </c>
+      <c r="C195" t="s">
+        <v>585</v>
+      </c>
+      <c r="D195">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>529</v>
+      </c>
+      <c r="B196" t="s">
+        <v>531</v>
+      </c>
+      <c r="C196" t="s">
+        <v>586</v>
+      </c>
+      <c r="D196">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>532</v>
+      </c>
+      <c r="B197" t="s">
+        <v>530</v>
+      </c>
+      <c r="C197" t="s">
+        <v>587</v>
+      </c>
+      <c r="D197">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B198" t="s">
+        <v>533</v>
+      </c>
+      <c r="C198" t="s">
+        <v>588</v>
+      </c>
+      <c r="D198">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>534</v>
+      </c>
+      <c r="B199" t="s">
+        <v>535</v>
+      </c>
+      <c r="C199" t="s">
+        <v>589</v>
+      </c>
+      <c r="D199">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>536</v>
+      </c>
+      <c r="B200" t="s">
+        <v>537</v>
+      </c>
+      <c r="C200" t="s">
+        <v>590</v>
+      </c>
+      <c r="D200">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>538</v>
+      </c>
+      <c r="B201" t="s">
+        <v>539</v>
+      </c>
+      <c r="C201" t="s">
+        <v>591</v>
+      </c>
+      <c r="D201">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>540</v>
+      </c>
+      <c r="B202" t="s">
+        <v>542</v>
+      </c>
+      <c r="C202" t="s">
+        <v>580</v>
+      </c>
+      <c r="D202">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>543</v>
+      </c>
+      <c r="B203" t="s">
+        <v>544</v>
+      </c>
+      <c r="C203" t="s">
+        <v>592</v>
+      </c>
+      <c r="D203">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>